<commit_message>
Update the results of round of 16
</commit_message>
<xml_diff>
--- a/input/r16/world_cup_2018r16_final.xlsx
+++ b/input/r16/world_cup_2018r16_final.xlsx
@@ -25,7 +25,7 @@
     <definedName name="T">T!$1:$1048576</definedName>
     <definedName name="teams">Settings!$I$17:$I$48</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -9322,6 +9322,90 @@
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -9400,90 +9484,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -29902,8 +29902,8 @@
   </sheetPr>
   <dimension ref="A1:BT97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="BA30" sqref="BA30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="BB39" sqref="BB39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -29958,25 +29958,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="str">
+      <c r="A1" s="136" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
       <c r="U1" s="58"/>
@@ -30039,11 +30039,11 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="116" t="str">
+      <c r="O3" s="137" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="116"/>
+      <c r="P3" s="137"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -30069,43 +30069,43 @@
     </row>
     <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="117" t="str">
+      <c r="A5" s="138" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="119"/>
-      <c r="J5" s="123" t="s">
+      <c r="B5" s="139"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="140"/>
+      <c r="J5" s="144" t="s">
         <v>2174</v>
       </c>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="125"/>
+      <c r="K5" s="145"/>
+      <c r="L5" s="145"/>
+      <c r="M5" s="145"/>
+      <c r="N5" s="145"/>
+      <c r="O5" s="145"/>
+      <c r="P5" s="146"/>
     </row>
     <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="122"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="127"/>
-      <c r="P6" s="128"/>
+      <c r="A6" s="141"/>
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="143"/>
+      <c r="J6" s="147"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="148"/>
+      <c r="P6" s="149"/>
       <c r="R6" s="58" t="s">
         <v>2175</v>
       </c>
@@ -30169,34 +30169,34 @@
       <c r="AT6" s="62" t="s">
         <v>2182</v>
       </c>
-      <c r="AY6" s="109" t="str">
+      <c r="AY6" s="130" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="AZ6" s="110"/>
-      <c r="BA6" s="110"/>
-      <c r="BB6" s="111"/>
-      <c r="BE6" s="109" t="str">
+      <c r="AZ6" s="131"/>
+      <c r="BA6" s="131"/>
+      <c r="BB6" s="132"/>
+      <c r="BE6" s="130" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BF6" s="110"/>
-      <c r="BG6" s="110"/>
-      <c r="BH6" s="111"/>
-      <c r="BK6" s="109" t="str">
+      <c r="BF6" s="131"/>
+      <c r="BG6" s="131"/>
+      <c r="BH6" s="132"/>
+      <c r="BK6" s="130" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BL6" s="110"/>
-      <c r="BM6" s="110"/>
-      <c r="BN6" s="111"/>
-      <c r="BQ6" s="109" t="str">
+      <c r="BL6" s="131"/>
+      <c r="BM6" s="131"/>
+      <c r="BN6" s="132"/>
+      <c r="BQ6" s="130" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BR6" s="110"/>
-      <c r="BS6" s="110"/>
-      <c r="BT6" s="111"/>
+      <c r="BR6" s="131"/>
+      <c r="BS6" s="131"/>
+      <c r="BT6" s="132"/>
     </row>
     <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
@@ -30260,22 +30260,22 @@
         <f>IF(OR(F7="",G7=""),"",IF(F7&gt;G7,1,IF(F7&lt;G7,-1,0)))</f>
         <v>1</v>
       </c>
-      <c r="AY7" s="112"/>
-      <c r="AZ7" s="113"/>
-      <c r="BA7" s="113"/>
-      <c r="BB7" s="114"/>
-      <c r="BE7" s="112"/>
-      <c r="BF7" s="113"/>
-      <c r="BG7" s="113"/>
-      <c r="BH7" s="114"/>
-      <c r="BK7" s="112"/>
-      <c r="BL7" s="113"/>
-      <c r="BM7" s="113"/>
-      <c r="BN7" s="114"/>
-      <c r="BQ7" s="112"/>
-      <c r="BR7" s="113"/>
-      <c r="BS7" s="113"/>
-      <c r="BT7" s="114"/>
+      <c r="AY7" s="133"/>
+      <c r="AZ7" s="134"/>
+      <c r="BA7" s="134"/>
+      <c r="BB7" s="135"/>
+      <c r="BE7" s="133"/>
+      <c r="BF7" s="134"/>
+      <c r="BG7" s="134"/>
+      <c r="BH7" s="135"/>
+      <c r="BK7" s="133"/>
+      <c r="BL7" s="134"/>
+      <c r="BM7" s="134"/>
+      <c r="BN7" s="135"/>
+      <c r="BQ7" s="133"/>
+      <c r="BR7" s="134"/>
+      <c r="BS7" s="134"/>
+      <c r="BT7" s="135"/>
     </row>
     <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
@@ -30821,7 +30821,7 @@
         <f>AR10-AS10</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="129">
+      <c r="AY10" s="118">
         <v>49</v>
       </c>
       <c r="AZ10" s="28" t="str">
@@ -31017,7 +31017,7 @@
         <f>AR11-AS11</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="130"/>
+      <c r="AY11" s="119"/>
       <c r="AZ11" s="31" t="str">
         <f>AO15</f>
         <v>Portugal</v>
@@ -31200,7 +31200,7 @@
       <c r="BB12" s="25"/>
       <c r="BC12" s="36"/>
       <c r="BD12" s="25"/>
-      <c r="BE12" s="129">
+      <c r="BE12" s="118">
         <v>57</v>
       </c>
       <c r="BF12" s="28" t="str">
@@ -31308,7 +31308,7 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="36"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="130"/>
+      <c r="BE13" s="119"/>
       <c r="BF13" s="31" t="str">
         <f>T59</f>
         <v>France</v>
@@ -31498,7 +31498,7 @@
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="129">
+      <c r="AY14" s="118">
         <v>50</v>
       </c>
       <c r="AZ14" s="28" t="str">
@@ -31698,7 +31698,7 @@
         <f>AR15-AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="130"/>
+      <c r="AY15" s="119"/>
       <c r="AZ15" s="31" t="str">
         <f>AO27</f>
         <v>Argentina</v>
@@ -31907,7 +31907,7 @@
       <c r="BH16" s="25"/>
       <c r="BI16" s="36"/>
       <c r="BJ16" s="25"/>
-      <c r="BK16" s="129">
+      <c r="BK16" s="118">
         <v>61</v>
       </c>
       <c r="BL16" s="28" t="str">
@@ -32104,7 +32104,7 @@
       <c r="BH17" s="25"/>
       <c r="BI17" s="36"/>
       <c r="BJ17" s="39"/>
-      <c r="BK17" s="130"/>
+      <c r="BK17" s="119"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
         <v>W58</v>
@@ -32264,14 +32264,16 @@
         <f>MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
         <v>1</v>
       </c>
-      <c r="AY18" s="129">
+      <c r="AY18" s="118">
         <v>53</v>
       </c>
       <c r="AZ18" s="28" t="str">
         <f>AO32</f>
         <v>Brazil</v>
       </c>
-      <c r="BA18" s="29"/>
+      <c r="BA18" s="29">
+        <v>2</v>
+      </c>
       <c r="BB18" s="30"/>
       <c r="BC18" s="25"/>
       <c r="BD18" s="25"/>
@@ -32369,12 +32371,14 @@
         <f>MIN(AI14:AI17)</f>
         <v>-2</v>
       </c>
-      <c r="AY19" s="130"/>
+      <c r="AY19" s="119"/>
       <c r="AZ19" s="31" t="str">
         <f>AO39</f>
         <v>Mexico</v>
       </c>
-      <c r="BA19" s="32"/>
+      <c r="BA19" s="32">
+        <v>0</v>
+      </c>
       <c r="BB19" s="33"/>
       <c r="BC19" s="34"/>
       <c r="BD19" s="25"/>
@@ -32574,12 +32578,12 @@
       <c r="BB20" s="25"/>
       <c r="BC20" s="36"/>
       <c r="BD20" s="25"/>
-      <c r="BE20" s="129">
+      <c r="BE20" s="118">
         <v>58</v>
       </c>
       <c r="BF20" s="28" t="str">
         <f>T62</f>
-        <v>W53</v>
+        <v>Brazil</v>
       </c>
       <c r="BG20" s="29"/>
       <c r="BH20" s="30"/>
@@ -32775,10 +32779,10 @@
       <c r="BB21" s="35"/>
       <c r="BC21" s="36"/>
       <c r="BD21" s="39"/>
-      <c r="BE21" s="130"/>
+      <c r="BE21" s="119"/>
       <c r="BF21" s="31" t="str">
         <f>T63</f>
-        <v>W54</v>
+        <v>Belgium</v>
       </c>
       <c r="BG21" s="32"/>
       <c r="BH21" s="33"/>
@@ -32961,14 +32965,16 @@
         <f>AR22-AS22</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="129">
+      <c r="AY22" s="118">
         <v>54</v>
       </c>
       <c r="AZ22" s="28" t="str">
         <f>AO44</f>
         <v>Belgium</v>
       </c>
-      <c r="BA22" s="29"/>
+      <c r="BA22" s="29">
+        <v>3</v>
+      </c>
       <c r="BB22" s="30"/>
       <c r="BC22" s="40"/>
       <c r="BD22" s="25"/>
@@ -33158,12 +33164,14 @@
         <f>AR23-AS23</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="130"/>
+      <c r="AY23" s="119"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
         <v>Japan</v>
       </c>
-      <c r="BA23" s="32"/>
+      <c r="BA23" s="32">
+        <v>2</v>
+      </c>
       <c r="BB23" s="33"/>
       <c r="BC23" s="25"/>
       <c r="BD23" s="25"/>
@@ -33179,7 +33187,7 @@
       <c r="BN23" s="25"/>
       <c r="BO23" s="36"/>
       <c r="BP23" s="25"/>
-      <c r="BQ23" s="129">
+      <c r="BQ23" s="118">
         <v>64</v>
       </c>
       <c r="BR23" s="28" t="str">
@@ -33352,7 +33360,7 @@
       <c r="BN24" s="25"/>
       <c r="BO24" s="36"/>
       <c r="BP24" s="39"/>
-      <c r="BQ24" s="130"/>
+      <c r="BQ24" s="119"/>
       <c r="BR24" s="31" t="str">
         <f>T77</f>
         <v>W62</v>
@@ -33633,7 +33641,7 @@
         <f>AR26-AS26</f>
         <v>0</v>
       </c>
-      <c r="AY26" s="129">
+      <c r="AY26" s="118">
         <v>51</v>
       </c>
       <c r="AZ26" s="28" t="str">
@@ -33835,7 +33843,7 @@
         <f>AR27-AS27</f>
         <v>0</v>
       </c>
-      <c r="AY27" s="130"/>
+      <c r="AY27" s="119"/>
       <c r="AZ27" s="31" t="str">
         <f>AO9</f>
         <v>Russia</v>
@@ -34040,7 +34048,7 @@
       <c r="BB28" s="25"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="25"/>
-      <c r="BE28" s="129">
+      <c r="BE28" s="118">
         <v>59</v>
       </c>
       <c r="BF28" s="28" t="str">
@@ -34237,7 +34245,7 @@
       <c r="BB29" s="35"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="39"/>
-      <c r="BE29" s="130"/>
+      <c r="BE29" s="119"/>
       <c r="BF29" s="31" t="str">
         <f>T61</f>
         <v>Croatia</v>
@@ -34403,7 +34411,7 @@
         <f>MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
         <v>1</v>
       </c>
-      <c r="AY30" s="129">
+      <c r="AY30" s="118">
         <v>52</v>
       </c>
       <c r="AZ30" s="28" t="str">
@@ -34505,7 +34513,7 @@
         <f>MIN(AI26:AI29)</f>
         <v>-3</v>
       </c>
-      <c r="AY31" s="130"/>
+      <c r="AY31" s="119"/>
       <c r="AZ31" s="31" t="str">
         <f>AO21</f>
         <v>Denmark</v>
@@ -34533,13 +34541,13 @@
       <c r="BN31" s="35"/>
       <c r="BO31" s="36"/>
       <c r="BP31" s="41"/>
-      <c r="BQ31" s="131" t="str">
+      <c r="BQ31" s="124" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BR31" s="132"/>
-      <c r="BS31" s="132"/>
-      <c r="BT31" s="133"/>
+      <c r="BR31" s="125"/>
+      <c r="BS31" s="125"/>
+      <c r="BT31" s="126"/>
     </row>
     <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
@@ -34723,7 +34731,7 @@
       <c r="BH32" s="25"/>
       <c r="BI32" s="36"/>
       <c r="BJ32" s="25"/>
-      <c r="BK32" s="129">
+      <c r="BK32" s="118">
         <v>62</v>
       </c>
       <c r="BL32" s="28" t="str">
@@ -34734,10 +34742,10 @@
       <c r="BN32" s="30"/>
       <c r="BO32" s="40"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="134"/>
-      <c r="BR32" s="135"/>
-      <c r="BS32" s="135"/>
-      <c r="BT32" s="136"/>
+      <c r="BQ32" s="127"/>
+      <c r="BR32" s="128"/>
+      <c r="BS32" s="128"/>
+      <c r="BT32" s="129"/>
     </row>
     <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -34924,7 +34932,7 @@
       <c r="BH33" s="25"/>
       <c r="BI33" s="36"/>
       <c r="BJ33" s="39"/>
-      <c r="BK33" s="130"/>
+      <c r="BK33" s="119"/>
       <c r="BL33" s="31" t="str">
         <f>T72</f>
         <v>W60</v>
@@ -35104,14 +35112,16 @@
         <f>AR34-AS34</f>
         <v>0</v>
       </c>
-      <c r="AY34" s="129">
+      <c r="AY34" s="118">
         <v>55</v>
       </c>
       <c r="AZ34" s="28" t="str">
         <f>AO38</f>
         <v>Sweden</v>
       </c>
-      <c r="BA34" s="29"/>
+      <c r="BA34" s="29">
+        <v>1</v>
+      </c>
       <c r="BB34" s="30"/>
       <c r="BC34" s="25"/>
       <c r="BD34" s="25"/>
@@ -35301,12 +35311,14 @@
         <f>AR35-AS35</f>
         <v>0</v>
       </c>
-      <c r="AY35" s="130"/>
+      <c r="AY35" s="119"/>
       <c r="AZ35" s="31" t="str">
         <f>AO33</f>
         <v>Switzerland</v>
       </c>
-      <c r="BA35" s="32"/>
+      <c r="BA35" s="32">
+        <v>0</v>
+      </c>
       <c r="BB35" s="33"/>
       <c r="BC35" s="34"/>
       <c r="BD35" s="25"/>
@@ -35325,7 +35337,7 @@
       <c r="BN35" s="25"/>
       <c r="BO35" s="25"/>
       <c r="BP35" s="25"/>
-      <c r="BQ35" s="129">
+      <c r="BQ35" s="118">
         <v>63</v>
       </c>
       <c r="BR35" s="28" t="str">
@@ -35487,12 +35499,12 @@
       <c r="BB36" s="25"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="25"/>
-      <c r="BE36" s="129">
+      <c r="BE36" s="118">
         <v>60</v>
       </c>
       <c r="BF36" s="28" t="str">
         <f>T64</f>
-        <v>W55</v>
+        <v>Sweden</v>
       </c>
       <c r="BG36" s="29"/>
       <c r="BH36" s="30"/>
@@ -35504,7 +35516,7 @@
       <c r="BN36" s="25"/>
       <c r="BO36" s="25"/>
       <c r="BP36" s="25"/>
-      <c r="BQ36" s="130"/>
+      <c r="BQ36" s="119"/>
       <c r="BR36" s="31" t="str">
         <f>Z77</f>
         <v>L62</v>
@@ -35591,10 +35603,10 @@
       <c r="BB37" s="35"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="39"/>
-      <c r="BE37" s="130"/>
+      <c r="BE37" s="119"/>
       <c r="BF37" s="31" t="str">
         <f>T65</f>
-        <v>W56</v>
+        <v>England</v>
       </c>
       <c r="BG37" s="32"/>
       <c r="BH37" s="33"/>
@@ -35781,15 +35793,19 @@
         <f>AR38-AS38</f>
         <v>0</v>
       </c>
-      <c r="AY38" s="129">
+      <c r="AY38" s="118">
         <v>56</v>
       </c>
       <c r="AZ38" s="28" t="str">
         <f>AO50</f>
         <v>Colombia</v>
       </c>
-      <c r="BA38" s="29"/>
-      <c r="BB38" s="30"/>
+      <c r="BA38" s="29">
+        <v>1</v>
+      </c>
+      <c r="BB38" s="30">
+        <v>3</v>
+      </c>
       <c r="BC38" s="40"/>
       <c r="BD38" s="25"/>
       <c r="BI38" s="25"/>
@@ -35975,13 +35991,17 @@
         <f>AR39-AS39</f>
         <v>0</v>
       </c>
-      <c r="AY39" s="130"/>
+      <c r="AY39" s="119"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
         <v>England</v>
       </c>
-      <c r="BA39" s="32"/>
-      <c r="BB39" s="33"/>
+      <c r="BA39" s="32">
+        <v>1</v>
+      </c>
+      <c r="BB39" s="33">
+        <v>4</v>
+      </c>
       <c r="BC39" s="25"/>
       <c r="BD39" s="25"/>
       <c r="BK39" s="25"/>
@@ -36328,23 +36348,23 @@
         <f>AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="146" t="str">
+      <c r="BJ41" s="120" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BK41" s="146"/>
-      <c r="BL41" s="146"/>
-      <c r="BM41" s="146"/>
-      <c r="BN41" s="146"/>
-      <c r="BO41" s="148" t="str">
+      <c r="BK41" s="120"/>
+      <c r="BL41" s="120"/>
+      <c r="BM41" s="120"/>
+      <c r="BN41" s="120"/>
+      <c r="BO41" s="122" t="str">
         <f>S85</f>
         <v/>
       </c>
-      <c r="BP41" s="148"/>
-      <c r="BQ41" s="148"/>
-      <c r="BR41" s="148"/>
-      <c r="BS41" s="148"/>
-      <c r="BT41" s="148"/>
+      <c r="BP41" s="122"/>
+      <c r="BQ41" s="122"/>
+      <c r="BR41" s="122"/>
+      <c r="BS41" s="122"/>
+      <c r="BT41" s="122"/>
     </row>
     <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -36492,17 +36512,17 @@
         <f>MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>1</v>
       </c>
-      <c r="BJ42" s="147"/>
-      <c r="BK42" s="147"/>
-      <c r="BL42" s="147"/>
-      <c r="BM42" s="147"/>
-      <c r="BN42" s="147"/>
-      <c r="BO42" s="149"/>
-      <c r="BP42" s="149"/>
-      <c r="BQ42" s="149"/>
-      <c r="BR42" s="149"/>
-      <c r="BS42" s="149"/>
-      <c r="BT42" s="149"/>
+      <c r="BJ42" s="121"/>
+      <c r="BK42" s="121"/>
+      <c r="BL42" s="121"/>
+      <c r="BM42" s="121"/>
+      <c r="BN42" s="121"/>
+      <c r="BO42" s="123"/>
+      <c r="BP42" s="123"/>
+      <c r="BQ42" s="123"/>
+      <c r="BR42" s="123"/>
+      <c r="BS42" s="123"/>
+      <c r="BT42" s="123"/>
     </row>
     <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -37084,12 +37104,12 @@
         <f>AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="137" t="s">
+      <c r="AY46" s="109" t="s">
         <v>2224</v>
       </c>
-      <c r="AZ46" s="138"/>
-      <c r="BA46" s="138"/>
-      <c r="BB46" s="139"/>
+      <c r="AZ46" s="110"/>
+      <c r="BA46" s="110"/>
+      <c r="BB46" s="111"/>
     </row>
     <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
@@ -37257,10 +37277,10 @@
         <f>AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="140"/>
-      <c r="AZ47" s="141"/>
-      <c r="BA47" s="141"/>
-      <c r="BB47" s="142"/>
+      <c r="AY47" s="112"/>
+      <c r="AZ47" s="113"/>
+      <c r="BA47" s="113"/>
+      <c r="BB47" s="114"/>
     </row>
     <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
@@ -37408,10 +37428,10 @@
         <f>MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="140"/>
-      <c r="AZ48" s="141"/>
-      <c r="BA48" s="141"/>
-      <c r="BB48" s="142"/>
+      <c r="AY48" s="112"/>
+      <c r="AZ48" s="113"/>
+      <c r="BA48" s="113"/>
+      <c r="BB48" s="114"/>
     </row>
     <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
@@ -37483,10 +37503,10 @@
         <f>MIN(AI44:AI47)</f>
         <v>-9</v>
       </c>
-      <c r="AY49" s="140"/>
-      <c r="AZ49" s="141"/>
-      <c r="BA49" s="141"/>
-      <c r="BB49" s="142"/>
+      <c r="AY49" s="112"/>
+      <c r="AZ49" s="113"/>
+      <c r="BA49" s="113"/>
+      <c r="BB49" s="114"/>
     </row>
     <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
@@ -37658,10 +37678,10 @@
         <f>AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="140"/>
-      <c r="AZ50" s="141"/>
-      <c r="BA50" s="141"/>
-      <c r="BB50" s="142"/>
+      <c r="AY50" s="112"/>
+      <c r="AZ50" s="113"/>
+      <c r="BA50" s="113"/>
+      <c r="BB50" s="114"/>
     </row>
     <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
@@ -37833,10 +37853,10 @@
         <f>AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="140"/>
-      <c r="AZ51" s="141"/>
-      <c r="BA51" s="141"/>
-      <c r="BB51" s="142"/>
+      <c r="AY51" s="112"/>
+      <c r="AZ51" s="113"/>
+      <c r="BA51" s="113"/>
+      <c r="BB51" s="114"/>
     </row>
     <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
@@ -38004,10 +38024,10 @@
         <f>AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="143"/>
-      <c r="AZ52" s="144"/>
-      <c r="BA52" s="144"/>
-      <c r="BB52" s="145"/>
+      <c r="AY52" s="115"/>
+      <c r="AZ52" s="116"/>
+      <c r="BA52" s="116"/>
+      <c r="BB52" s="117"/>
     </row>
     <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -38414,11 +38434,11 @@
       </c>
       <c r="S62" s="65" t="str">
         <f>IF(OR(BA18="",BA19=""),"",IF(BA18&gt;BA19,AZ18,IF(BA18&lt;BA19,AZ19,IF(OR(BB18="",BB19=""),"draw",IF(BB18&gt;BB19,AZ18,IF(BB18&lt;BB19,AZ19,"draw"))))))</f>
-        <v/>
+        <v>Brazil</v>
       </c>
       <c r="T62" s="65" t="str">
         <f>IF(OR(S62="",S62="draw"),INDEX(T,90,lang),S62)</f>
-        <v>W53</v>
+        <v>Brazil</v>
       </c>
     </row>
     <row r="63" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -38428,11 +38448,11 @@
       </c>
       <c r="S63" s="65" t="str">
         <f>IF(OR(BA22="",BA23=""),"",IF(BA22&gt;BA23,AZ22,IF(BA22&lt;BA23,AZ23,IF(OR(BB22="",BB23=""),"draw",IF(BB22&gt;BB23,AZ22,IF(BB22&lt;BB23,AZ23,"draw"))))))</f>
-        <v/>
+        <v>Belgium</v>
       </c>
       <c r="T63" s="65" t="str">
         <f>IF(OR(S63="",S63="draw"),INDEX(T,91,lang),S63)</f>
-        <v>W54</v>
+        <v>Belgium</v>
       </c>
     </row>
     <row r="64" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -38442,11 +38462,11 @@
       </c>
       <c r="S64" s="65" t="str">
         <f>IF(OR(BA34="",BA35=""),"",IF(BA34&gt;BA35,AZ34,IF(BA34&lt;BA35,AZ35,IF(OR(BB34="",BB35=""),"draw",IF(BB34&gt;BB35,AZ34,IF(BB34&lt;BB35,AZ35,"draw"))))))</f>
-        <v/>
+        <v>Sweden</v>
       </c>
       <c r="T64" s="65" t="str">
         <f>IF(OR(S64="",S64="draw"),INDEX(T,92,lang),S64)</f>
-        <v>W55</v>
+        <v>Sweden</v>
       </c>
     </row>
     <row r="65" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -38456,11 +38476,11 @@
       </c>
       <c r="S65" s="65" t="str">
         <f>IF(OR(BA38="",BA39=""),"",IF(BA38&gt;BA39,AZ38,IF(BA38&lt;BA39,AZ39,IF(OR(BB38="",BB39=""),"draw",IF(BB38&gt;BB39,AZ38,IF(BB38&lt;BB39,AZ39,"draw"))))))</f>
-        <v/>
+        <v>England</v>
       </c>
       <c r="T65" s="65" t="str">
         <f>IF(OR(S65="",S65="draw"),INDEX(T,93,lang),S65)</f>
-        <v>W56</v>
+        <v>England</v>
       </c>
     </row>
     <row r="66" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -38604,6 +38624,27 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="hexNDhodxxdoIYhe+LOVPFyB2v0aJLQphXCm5lZGwHDaP2ZITl3Lpck5mriyKWgCt8wrzYbwlizwv7dyeeElyw==" saltValue="swcCixFXOL0FnpwQehLBng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
+    <mergeCell ref="BQ6:BT7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
+    <mergeCell ref="AY10:AY11"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="AY6:BB7"/>
+    <mergeCell ref="BE6:BH7"/>
+    <mergeCell ref="BK6:BN7"/>
+    <mergeCell ref="AY22:AY23"/>
+    <mergeCell ref="BQ23:BQ24"/>
+    <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="BE20:BE21"/>
+    <mergeCell ref="AY14:AY15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="AY30:AY31"/>
+    <mergeCell ref="BQ31:BT32"/>
+    <mergeCell ref="BK32:BK33"/>
+    <mergeCell ref="AY26:AY27"/>
+    <mergeCell ref="BE28:BE29"/>
     <mergeCell ref="AY46:BB52"/>
     <mergeCell ref="AY38:AY39"/>
     <mergeCell ref="BJ41:BN42"/>
@@ -38611,27 +38652,6 @@
     <mergeCell ref="BQ35:BQ36"/>
     <mergeCell ref="BE36:BE37"/>
     <mergeCell ref="BO41:BT42"/>
-    <mergeCell ref="AY30:AY31"/>
-    <mergeCell ref="BQ31:BT32"/>
-    <mergeCell ref="BK32:BK33"/>
-    <mergeCell ref="AY26:AY27"/>
-    <mergeCell ref="BE28:BE29"/>
-    <mergeCell ref="AY22:AY23"/>
-    <mergeCell ref="BQ23:BQ24"/>
-    <mergeCell ref="AY18:AY19"/>
-    <mergeCell ref="BE20:BE21"/>
-    <mergeCell ref="AY14:AY15"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="AY10:AY11"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="AY6:BB7"/>
-    <mergeCell ref="BE6:BH7"/>
-    <mergeCell ref="BK6:BN7"/>
-    <mergeCell ref="BQ6:BT7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="F7:F55">

</xml_diff>

<commit_message>
Update the latest games
</commit_message>
<xml_diff>
--- a/input/r16/world_cup_2018r16_final.xlsx
+++ b/input/r16/world_cup_2018r16_final.xlsx
@@ -29903,7 +29903,7 @@
   <dimension ref="A1:BT97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="BB39" sqref="BB39"/>
+      <selection activeCell="BG24" sqref="BG24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -31207,7 +31207,9 @@
         <f>T58</f>
         <v>Uruguay</v>
       </c>
-      <c r="BG12" s="29"/>
+      <c r="BG12" s="29">
+        <v>0</v>
+      </c>
       <c r="BH12" s="30"/>
       <c r="BI12" s="25"/>
       <c r="BJ12" s="25"/>
@@ -31313,7 +31315,9 @@
         <f>T59</f>
         <v>France</v>
       </c>
-      <c r="BG13" s="32"/>
+      <c r="BG13" s="32">
+        <v>2</v>
+      </c>
       <c r="BH13" s="33"/>
       <c r="BI13" s="34"/>
       <c r="BJ13" s="25"/>
@@ -31912,7 +31916,7 @@
       </c>
       <c r="BL16" s="28" t="str">
         <f>T69</f>
-        <v>W57</v>
+        <v>France</v>
       </c>
       <c r="BM16" s="29"/>
       <c r="BN16" s="30"/>
@@ -32107,7 +32111,7 @@
       <c r="BK17" s="119"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
-        <v>W58</v>
+        <v>Belgium</v>
       </c>
       <c r="BM17" s="32"/>
       <c r="BN17" s="33"/>
@@ -32585,7 +32589,9 @@
         <f>T62</f>
         <v>Brazil</v>
       </c>
-      <c r="BG20" s="29"/>
+      <c r="BG20" s="29">
+        <v>1</v>
+      </c>
       <c r="BH20" s="30"/>
       <c r="BI20" s="40"/>
       <c r="BJ20" s="25"/>
@@ -32784,7 +32790,9 @@
         <f>T63</f>
         <v>Belgium</v>
       </c>
-      <c r="BG21" s="32"/>
+      <c r="BG21" s="32">
+        <v>2</v>
+      </c>
       <c r="BH21" s="33"/>
       <c r="BI21" s="25"/>
       <c r="BJ21" s="25"/>
@@ -38493,11 +38501,11 @@
       </c>
       <c r="S69" s="65" t="str">
         <f>IF(OR(BG12="",BG13=""),"",IF(BG12&gt;BG13,BF12,IF(BG12&lt;BG13,BF13,IF(OR(BH12="",BH13=""),"draw",IF(BH12&gt;BH13,BF12,IF(BH12&lt;BH13,BF13,"draw"))))))</f>
-        <v/>
+        <v>France</v>
       </c>
       <c r="T69" s="65" t="str">
         <f>IF(OR(S69="",S69="draw"),INDEX(T,94,lang),S69)</f>
-        <v>W57</v>
+        <v>France</v>
       </c>
     </row>
     <row r="70" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -38507,11 +38515,11 @@
       </c>
       <c r="S70" s="65" t="str">
         <f>IF(OR(BG20="",BG21=""),"",IF(BG20&gt;BG21,BF20,IF(BG20&lt;BG21,BF21,IF(OR(BH20="",BH21=""),"draw",IF(BH20&gt;BH21,BF20,IF(BH20&lt;BH21,BF21,"draw"))))))</f>
-        <v/>
+        <v>Belgium</v>
       </c>
       <c r="T70" s="65" t="str">
         <f>IF(OR(S70="",S70="draw"),INDEX(T,95,lang),S70)</f>
-        <v>W58</v>
+        <v>Belgium</v>
       </c>
     </row>
     <row r="71" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update for quarter final
</commit_message>
<xml_diff>
--- a/input/r16/world_cup_2018r16_final.xlsx
+++ b/input/r16/world_cup_2018r16_final.xlsx
@@ -9322,90 +9322,6 @@
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -9484,6 +9400,90 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -29902,8 +29902,8 @@
   </sheetPr>
   <dimension ref="A1:BT97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="BG24" sqref="BG24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E9" workbookViewId="0">
+      <selection activeCell="BH22" sqref="BH22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -29958,25 +29958,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="str">
+      <c r="A1" s="115" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
       <c r="U1" s="58"/>
@@ -30039,11 +30039,11 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="137" t="str">
+      <c r="O3" s="116" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="137"/>
+      <c r="P3" s="116"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -30069,43 +30069,43 @@
     </row>
     <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="138" t="str">
+      <c r="A5" s="117" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
-      <c r="J5" s="144" t="s">
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="119"/>
+      <c r="J5" s="123" t="s">
         <v>2174</v>
       </c>
-      <c r="K5" s="145"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="146"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="125"/>
     </row>
     <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="141"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="149"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="128"/>
       <c r="R6" s="58" t="s">
         <v>2175</v>
       </c>
@@ -30169,34 +30169,34 @@
       <c r="AT6" s="62" t="s">
         <v>2182</v>
       </c>
-      <c r="AY6" s="130" t="str">
+      <c r="AY6" s="109" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="AZ6" s="131"/>
-      <c r="BA6" s="131"/>
-      <c r="BB6" s="132"/>
-      <c r="BE6" s="130" t="str">
+      <c r="AZ6" s="110"/>
+      <c r="BA6" s="110"/>
+      <c r="BB6" s="111"/>
+      <c r="BE6" s="109" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BF6" s="131"/>
-      <c r="BG6" s="131"/>
-      <c r="BH6" s="132"/>
-      <c r="BK6" s="130" t="str">
+      <c r="BF6" s="110"/>
+      <c r="BG6" s="110"/>
+      <c r="BH6" s="111"/>
+      <c r="BK6" s="109" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BL6" s="131"/>
-      <c r="BM6" s="131"/>
-      <c r="BN6" s="132"/>
-      <c r="BQ6" s="130" t="str">
+      <c r="BL6" s="110"/>
+      <c r="BM6" s="110"/>
+      <c r="BN6" s="111"/>
+      <c r="BQ6" s="109" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BR6" s="131"/>
-      <c r="BS6" s="131"/>
-      <c r="BT6" s="132"/>
+      <c r="BR6" s="110"/>
+      <c r="BS6" s="110"/>
+      <c r="BT6" s="111"/>
     </row>
     <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
@@ -30260,22 +30260,22 @@
         <f>IF(OR(F7="",G7=""),"",IF(F7&gt;G7,1,IF(F7&lt;G7,-1,0)))</f>
         <v>1</v>
       </c>
-      <c r="AY7" s="133"/>
-      <c r="AZ7" s="134"/>
-      <c r="BA7" s="134"/>
-      <c r="BB7" s="135"/>
-      <c r="BE7" s="133"/>
-      <c r="BF7" s="134"/>
-      <c r="BG7" s="134"/>
-      <c r="BH7" s="135"/>
-      <c r="BK7" s="133"/>
-      <c r="BL7" s="134"/>
-      <c r="BM7" s="134"/>
-      <c r="BN7" s="135"/>
-      <c r="BQ7" s="133"/>
-      <c r="BR7" s="134"/>
-      <c r="BS7" s="134"/>
-      <c r="BT7" s="135"/>
+      <c r="AY7" s="112"/>
+      <c r="AZ7" s="113"/>
+      <c r="BA7" s="113"/>
+      <c r="BB7" s="114"/>
+      <c r="BE7" s="112"/>
+      <c r="BF7" s="113"/>
+      <c r="BG7" s="113"/>
+      <c r="BH7" s="114"/>
+      <c r="BK7" s="112"/>
+      <c r="BL7" s="113"/>
+      <c r="BM7" s="113"/>
+      <c r="BN7" s="114"/>
+      <c r="BQ7" s="112"/>
+      <c r="BR7" s="113"/>
+      <c r="BS7" s="113"/>
+      <c r="BT7" s="114"/>
     </row>
     <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
@@ -30821,7 +30821,7 @@
         <f>AR10-AS10</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="118">
+      <c r="AY10" s="129">
         <v>49</v>
       </c>
       <c r="AZ10" s="28" t="str">
@@ -31017,7 +31017,7 @@
         <f>AR11-AS11</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="119"/>
+      <c r="AY11" s="130"/>
       <c r="AZ11" s="31" t="str">
         <f>AO15</f>
         <v>Portugal</v>
@@ -31200,7 +31200,7 @@
       <c r="BB12" s="25"/>
       <c r="BC12" s="36"/>
       <c r="BD12" s="25"/>
-      <c r="BE12" s="118">
+      <c r="BE12" s="129">
         <v>57</v>
       </c>
       <c r="BF12" s="28" t="str">
@@ -31310,7 +31310,7 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="36"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="119"/>
+      <c r="BE13" s="130"/>
       <c r="BF13" s="31" t="str">
         <f>T59</f>
         <v>France</v>
@@ -31502,7 +31502,7 @@
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="118">
+      <c r="AY14" s="129">
         <v>50</v>
       </c>
       <c r="AZ14" s="28" t="str">
@@ -31702,7 +31702,7 @@
         <f>AR15-AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="119"/>
+      <c r="AY15" s="130"/>
       <c r="AZ15" s="31" t="str">
         <f>AO27</f>
         <v>Argentina</v>
@@ -31911,7 +31911,7 @@
       <c r="BH16" s="25"/>
       <c r="BI16" s="36"/>
       <c r="BJ16" s="25"/>
-      <c r="BK16" s="118">
+      <c r="BK16" s="129">
         <v>61</v>
       </c>
       <c r="BL16" s="28" t="str">
@@ -32108,7 +32108,7 @@
       <c r="BH17" s="25"/>
       <c r="BI17" s="36"/>
       <c r="BJ17" s="39"/>
-      <c r="BK17" s="119"/>
+      <c r="BK17" s="130"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
         <v>Belgium</v>
@@ -32268,7 +32268,7 @@
         <f>MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
         <v>1</v>
       </c>
-      <c r="AY18" s="118">
+      <c r="AY18" s="129">
         <v>53</v>
       </c>
       <c r="AZ18" s="28" t="str">
@@ -32375,7 +32375,7 @@
         <f>MIN(AI14:AI17)</f>
         <v>-2</v>
       </c>
-      <c r="AY19" s="119"/>
+      <c r="AY19" s="130"/>
       <c r="AZ19" s="31" t="str">
         <f>AO39</f>
         <v>Mexico</v>
@@ -32582,7 +32582,7 @@
       <c r="BB20" s="25"/>
       <c r="BC20" s="36"/>
       <c r="BD20" s="25"/>
-      <c r="BE20" s="118">
+      <c r="BE20" s="129">
         <v>58</v>
       </c>
       <c r="BF20" s="28" t="str">
@@ -32785,7 +32785,7 @@
       <c r="BB21" s="35"/>
       <c r="BC21" s="36"/>
       <c r="BD21" s="39"/>
-      <c r="BE21" s="119"/>
+      <c r="BE21" s="130"/>
       <c r="BF21" s="31" t="str">
         <f>T63</f>
         <v>Belgium</v>
@@ -32973,7 +32973,7 @@
         <f>AR22-AS22</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="118">
+      <c r="AY22" s="129">
         <v>54</v>
       </c>
       <c r="AZ22" s="28" t="str">
@@ -33172,7 +33172,7 @@
         <f>AR23-AS23</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="119"/>
+      <c r="AY23" s="130"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
         <v>Japan</v>
@@ -33195,7 +33195,7 @@
       <c r="BN23" s="25"/>
       <c r="BO23" s="36"/>
       <c r="BP23" s="25"/>
-      <c r="BQ23" s="118">
+      <c r="BQ23" s="129">
         <v>64</v>
       </c>
       <c r="BR23" s="28" t="str">
@@ -33368,7 +33368,7 @@
       <c r="BN24" s="25"/>
       <c r="BO24" s="36"/>
       <c r="BP24" s="39"/>
-      <c r="BQ24" s="119"/>
+      <c r="BQ24" s="130"/>
       <c r="BR24" s="31" t="str">
         <f>T77</f>
         <v>W62</v>
@@ -33649,7 +33649,7 @@
         <f>AR26-AS26</f>
         <v>0</v>
       </c>
-      <c r="AY26" s="118">
+      <c r="AY26" s="129">
         <v>51</v>
       </c>
       <c r="AZ26" s="28" t="str">
@@ -33851,7 +33851,7 @@
         <f>AR27-AS27</f>
         <v>0</v>
       </c>
-      <c r="AY27" s="119"/>
+      <c r="AY27" s="130"/>
       <c r="AZ27" s="31" t="str">
         <f>AO9</f>
         <v>Russia</v>
@@ -34056,15 +34056,19 @@
       <c r="BB28" s="25"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="25"/>
-      <c r="BE28" s="118">
+      <c r="BE28" s="129">
         <v>59</v>
       </c>
       <c r="BF28" s="28" t="str">
         <f>T60</f>
         <v>Russia</v>
       </c>
-      <c r="BG28" s="29"/>
-      <c r="BH28" s="30"/>
+      <c r="BG28" s="29">
+        <v>2</v>
+      </c>
+      <c r="BH28" s="30">
+        <v>3</v>
+      </c>
       <c r="BI28" s="25"/>
       <c r="BJ28" s="25"/>
       <c r="BK28" s="25"/>
@@ -34253,13 +34257,17 @@
       <c r="BB29" s="35"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="39"/>
-      <c r="BE29" s="119"/>
+      <c r="BE29" s="130"/>
       <c r="BF29" s="31" t="str">
         <f>T61</f>
         <v>Croatia</v>
       </c>
-      <c r="BG29" s="32"/>
-      <c r="BH29" s="33"/>
+      <c r="BG29" s="32">
+        <v>2</v>
+      </c>
+      <c r="BH29" s="33">
+        <v>4</v>
+      </c>
       <c r="BI29" s="34"/>
       <c r="BJ29" s="25"/>
       <c r="BK29" s="25"/>
@@ -34419,7 +34427,7 @@
         <f>MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
         <v>1</v>
       </c>
-      <c r="AY30" s="118">
+      <c r="AY30" s="129">
         <v>52</v>
       </c>
       <c r="AZ30" s="28" t="str">
@@ -34521,7 +34529,7 @@
         <f>MIN(AI26:AI29)</f>
         <v>-3</v>
       </c>
-      <c r="AY31" s="119"/>
+      <c r="AY31" s="130"/>
       <c r="AZ31" s="31" t="str">
         <f>AO21</f>
         <v>Denmark</v>
@@ -34549,13 +34557,13 @@
       <c r="BN31" s="35"/>
       <c r="BO31" s="36"/>
       <c r="BP31" s="41"/>
-      <c r="BQ31" s="124" t="str">
+      <c r="BQ31" s="131" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BR31" s="125"/>
-      <c r="BS31" s="125"/>
-      <c r="BT31" s="126"/>
+      <c r="BR31" s="132"/>
+      <c r="BS31" s="132"/>
+      <c r="BT31" s="133"/>
     </row>
     <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
@@ -34739,21 +34747,21 @@
       <c r="BH32" s="25"/>
       <c r="BI32" s="36"/>
       <c r="BJ32" s="25"/>
-      <c r="BK32" s="118">
+      <c r="BK32" s="129">
         <v>62</v>
       </c>
       <c r="BL32" s="28" t="str">
         <f>T71</f>
-        <v>W59</v>
+        <v>Croatia</v>
       </c>
       <c r="BM32" s="29"/>
       <c r="BN32" s="30"/>
       <c r="BO32" s="40"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="127"/>
-      <c r="BR32" s="128"/>
-      <c r="BS32" s="128"/>
-      <c r="BT32" s="129"/>
+      <c r="BQ32" s="134"/>
+      <c r="BR32" s="135"/>
+      <c r="BS32" s="135"/>
+      <c r="BT32" s="136"/>
     </row>
     <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -34940,10 +34948,10 @@
       <c r="BH33" s="25"/>
       <c r="BI33" s="36"/>
       <c r="BJ33" s="39"/>
-      <c r="BK33" s="119"/>
+      <c r="BK33" s="130"/>
       <c r="BL33" s="31" t="str">
         <f>T72</f>
-        <v>W60</v>
+        <v>England</v>
       </c>
       <c r="BM33" s="32"/>
       <c r="BN33" s="33"/>
@@ -35120,7 +35128,7 @@
         <f>AR34-AS34</f>
         <v>0</v>
       </c>
-      <c r="AY34" s="118">
+      <c r="AY34" s="129">
         <v>55</v>
       </c>
       <c r="AZ34" s="28" t="str">
@@ -35319,7 +35327,7 @@
         <f>AR35-AS35</f>
         <v>0</v>
       </c>
-      <c r="AY35" s="119"/>
+      <c r="AY35" s="130"/>
       <c r="AZ35" s="31" t="str">
         <f>AO33</f>
         <v>Switzerland</v>
@@ -35345,7 +35353,7 @@
       <c r="BN35" s="25"/>
       <c r="BO35" s="25"/>
       <c r="BP35" s="25"/>
-      <c r="BQ35" s="118">
+      <c r="BQ35" s="129">
         <v>63</v>
       </c>
       <c r="BR35" s="28" t="str">
@@ -35507,14 +35515,16 @@
       <c r="BB36" s="25"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="25"/>
-      <c r="BE36" s="118">
+      <c r="BE36" s="129">
         <v>60</v>
       </c>
       <c r="BF36" s="28" t="str">
         <f>T64</f>
         <v>Sweden</v>
       </c>
-      <c r="BG36" s="29"/>
+      <c r="BG36" s="29">
+        <v>0</v>
+      </c>
       <c r="BH36" s="30"/>
       <c r="BI36" s="40"/>
       <c r="BJ36" s="25"/>
@@ -35524,7 +35534,7 @@
       <c r="BN36" s="25"/>
       <c r="BO36" s="25"/>
       <c r="BP36" s="25"/>
-      <c r="BQ36" s="119"/>
+      <c r="BQ36" s="130"/>
       <c r="BR36" s="31" t="str">
         <f>Z77</f>
         <v>L62</v>
@@ -35611,12 +35621,14 @@
       <c r="BB37" s="35"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="39"/>
-      <c r="BE37" s="119"/>
+      <c r="BE37" s="130"/>
       <c r="BF37" s="31" t="str">
         <f>T65</f>
         <v>England</v>
       </c>
-      <c r="BG37" s="32"/>
+      <c r="BG37" s="32">
+        <v>2</v>
+      </c>
       <c r="BH37" s="33"/>
       <c r="BI37" s="25"/>
       <c r="BJ37" s="25"/>
@@ -35801,7 +35813,7 @@
         <f>AR38-AS38</f>
         <v>0</v>
       </c>
-      <c r="AY38" s="118">
+      <c r="AY38" s="129">
         <v>56</v>
       </c>
       <c r="AZ38" s="28" t="str">
@@ -35999,7 +36011,7 @@
         <f>AR39-AS39</f>
         <v>0</v>
       </c>
-      <c r="AY39" s="119"/>
+      <c r="AY39" s="130"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
         <v>England</v>
@@ -36356,23 +36368,23 @@
         <f>AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="120" t="str">
+      <c r="BJ41" s="146" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BK41" s="120"/>
-      <c r="BL41" s="120"/>
-      <c r="BM41" s="120"/>
-      <c r="BN41" s="120"/>
-      <c r="BO41" s="122" t="str">
+      <c r="BK41" s="146"/>
+      <c r="BL41" s="146"/>
+      <c r="BM41" s="146"/>
+      <c r="BN41" s="146"/>
+      <c r="BO41" s="148" t="str">
         <f>S85</f>
         <v/>
       </c>
-      <c r="BP41" s="122"/>
-      <c r="BQ41" s="122"/>
-      <c r="BR41" s="122"/>
-      <c r="BS41" s="122"/>
-      <c r="BT41" s="122"/>
+      <c r="BP41" s="148"/>
+      <c r="BQ41" s="148"/>
+      <c r="BR41" s="148"/>
+      <c r="BS41" s="148"/>
+      <c r="BT41" s="148"/>
     </row>
     <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -36520,17 +36532,17 @@
         <f>MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>1</v>
       </c>
-      <c r="BJ42" s="121"/>
-      <c r="BK42" s="121"/>
-      <c r="BL42" s="121"/>
-      <c r="BM42" s="121"/>
-      <c r="BN42" s="121"/>
-      <c r="BO42" s="123"/>
-      <c r="BP42" s="123"/>
-      <c r="BQ42" s="123"/>
-      <c r="BR42" s="123"/>
-      <c r="BS42" s="123"/>
-      <c r="BT42" s="123"/>
+      <c r="BJ42" s="147"/>
+      <c r="BK42" s="147"/>
+      <c r="BL42" s="147"/>
+      <c r="BM42" s="147"/>
+      <c r="BN42" s="147"/>
+      <c r="BO42" s="149"/>
+      <c r="BP42" s="149"/>
+      <c r="BQ42" s="149"/>
+      <c r="BR42" s="149"/>
+      <c r="BS42" s="149"/>
+      <c r="BT42" s="149"/>
     </row>
     <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -37112,12 +37124,12 @@
         <f>AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="109" t="s">
+      <c r="AY46" s="137" t="s">
         <v>2224</v>
       </c>
-      <c r="AZ46" s="110"/>
-      <c r="BA46" s="110"/>
-      <c r="BB46" s="111"/>
+      <c r="AZ46" s="138"/>
+      <c r="BA46" s="138"/>
+      <c r="BB46" s="139"/>
     </row>
     <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
@@ -37285,10 +37297,10 @@
         <f>AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="112"/>
-      <c r="AZ47" s="113"/>
-      <c r="BA47" s="113"/>
-      <c r="BB47" s="114"/>
+      <c r="AY47" s="140"/>
+      <c r="AZ47" s="141"/>
+      <c r="BA47" s="141"/>
+      <c r="BB47" s="142"/>
     </row>
     <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
@@ -37436,10 +37448,10 @@
         <f>MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="112"/>
-      <c r="AZ48" s="113"/>
-      <c r="BA48" s="113"/>
-      <c r="BB48" s="114"/>
+      <c r="AY48" s="140"/>
+      <c r="AZ48" s="141"/>
+      <c r="BA48" s="141"/>
+      <c r="BB48" s="142"/>
     </row>
     <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
@@ -37511,10 +37523,10 @@
         <f>MIN(AI44:AI47)</f>
         <v>-9</v>
       </c>
-      <c r="AY49" s="112"/>
-      <c r="AZ49" s="113"/>
-      <c r="BA49" s="113"/>
-      <c r="BB49" s="114"/>
+      <c r="AY49" s="140"/>
+      <c r="AZ49" s="141"/>
+      <c r="BA49" s="141"/>
+      <c r="BB49" s="142"/>
     </row>
     <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
@@ -37686,10 +37698,10 @@
         <f>AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="112"/>
-      <c r="AZ50" s="113"/>
-      <c r="BA50" s="113"/>
-      <c r="BB50" s="114"/>
+      <c r="AY50" s="140"/>
+      <c r="AZ50" s="141"/>
+      <c r="BA50" s="141"/>
+      <c r="BB50" s="142"/>
     </row>
     <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
@@ -37861,10 +37873,10 @@
         <f>AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="112"/>
-      <c r="AZ51" s="113"/>
-      <c r="BA51" s="113"/>
-      <c r="BB51" s="114"/>
+      <c r="AY51" s="140"/>
+      <c r="AZ51" s="141"/>
+      <c r="BA51" s="141"/>
+      <c r="BB51" s="142"/>
     </row>
     <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
@@ -38032,10 +38044,10 @@
         <f>AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="115"/>
-      <c r="AZ52" s="116"/>
-      <c r="BA52" s="116"/>
-      <c r="BB52" s="117"/>
+      <c r="AY52" s="143"/>
+      <c r="AZ52" s="144"/>
+      <c r="BA52" s="144"/>
+      <c r="BB52" s="145"/>
     </row>
     <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -38529,11 +38541,11 @@
       </c>
       <c r="S71" s="65" t="str">
         <f>IF(OR(BG28="",BG29=""),"",IF(BG28&gt;BG29,BF28,IF(BG28&lt;BG29,BF29,IF(OR(BH28="",BH29=""),"draw",IF(BH28&gt;BH29,BF28,IF(BH28&lt;BH29,BF29,"draw"))))))</f>
-        <v/>
+        <v>Croatia</v>
       </c>
       <c r="T71" s="65" t="str">
         <f>IF(OR(S71="",S71="draw"),INDEX(T,96,lang),S71)</f>
-        <v>W59</v>
+        <v>Croatia</v>
       </c>
     </row>
     <row r="72" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -38543,11 +38555,11 @@
       </c>
       <c r="S72" s="65" t="str">
         <f>IF(OR(BG36="",BG37=""),"",IF(BG36&gt;BG37,BF36,IF(BG36&lt;BG37,BF37,IF(OR(BH36="",BH37=""),"draw",IF(BH36&gt;BH37,BF36,IF(BH36&lt;BH37,BF37,"draw"))))))</f>
-        <v/>
+        <v>England</v>
       </c>
       <c r="T72" s="65" t="str">
         <f>IF(OR(S72="",S72="draw"),INDEX(T,97,lang),S72)</f>
-        <v>W60</v>
+        <v>England</v>
       </c>
     </row>
     <row r="73" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -38632,27 +38644,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="hexNDhodxxdoIYhe+LOVPFyB2v0aJLQphXCm5lZGwHDaP2ZITl3Lpck5mriyKWgCt8wrzYbwlizwv7dyeeElyw==" saltValue="swcCixFXOL0FnpwQehLBng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="BQ6:BT7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
-    <mergeCell ref="AY10:AY11"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="AY6:BB7"/>
-    <mergeCell ref="BE6:BH7"/>
-    <mergeCell ref="BK6:BN7"/>
-    <mergeCell ref="AY22:AY23"/>
-    <mergeCell ref="BQ23:BQ24"/>
-    <mergeCell ref="AY18:AY19"/>
-    <mergeCell ref="BE20:BE21"/>
-    <mergeCell ref="AY14:AY15"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="AY30:AY31"/>
-    <mergeCell ref="BQ31:BT32"/>
-    <mergeCell ref="BK32:BK33"/>
-    <mergeCell ref="AY26:AY27"/>
-    <mergeCell ref="BE28:BE29"/>
     <mergeCell ref="AY46:BB52"/>
     <mergeCell ref="AY38:AY39"/>
     <mergeCell ref="BJ41:BN42"/>
@@ -38660,6 +38651,27 @@
     <mergeCell ref="BQ35:BQ36"/>
     <mergeCell ref="BE36:BE37"/>
     <mergeCell ref="BO41:BT42"/>
+    <mergeCell ref="AY30:AY31"/>
+    <mergeCell ref="BQ31:BT32"/>
+    <mergeCell ref="BK32:BK33"/>
+    <mergeCell ref="AY26:AY27"/>
+    <mergeCell ref="BE28:BE29"/>
+    <mergeCell ref="AY22:AY23"/>
+    <mergeCell ref="BQ23:BQ24"/>
+    <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="BE20:BE21"/>
+    <mergeCell ref="AY14:AY15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="AY10:AY11"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="AY6:BB7"/>
+    <mergeCell ref="BE6:BH7"/>
+    <mergeCell ref="BK6:BN7"/>
+    <mergeCell ref="BQ6:BT7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="F7:F55">

</xml_diff>